<commit_message>
Added em, ths and sina balance sheet examples
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF31B926-A3F4-48C5-AB17-03C015CB9D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="19140" windowHeight="10608"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="AvailableIndices" sheetId="2" r:id="rId2"/>
     <sheet name="BalanceSheetData" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,100 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Roger Ye:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>URL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>: https://site.financialmodelingprep.com/developer/docs#Historical-stock-index-prices
-[
- {
-  "symbol": "PRAA",
-  "name": "PRA Group, Inc.",
-  "currency": "USD",
-  "stockExchange": "NasdaqGS",
-  "exchangeShortName": "NASDAQ"
- },
- {
-  "symbol": "PAAS",
-  "name": "Pan American Silver Corp.",
-  "currency": "USD",
-  "stockExchange": "NasdaqGS",
-  "exchangeShortName": "NASDAQ"
- }
-]</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Roger Ye</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Roger Ye:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-name=S&amp;P 500 Index, currency=None, code=spx, symbol=^SPX</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -202,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="192">
   <si>
     <t>Model</t>
   </si>
@@ -295,17 +209,501 @@
   </si>
   <si>
     <t>Balance Sheet (资产负债表)</t>
+  </si>
+  <si>
+    <t>根据你提供的数据结构，以下是英文键（Key）与对应中文翻译的对照表格：</t>
+  </si>
+  <si>
+    <t>英文 Key</t>
+  </si>
+  <si>
+    <t>中文 Key</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>股票代码</t>
+  </si>
+  <si>
+    <t>reportedCurrency</t>
+  </si>
+  <si>
+    <t>报告货币</t>
+  </si>
+  <si>
+    <t>cik</t>
+  </si>
+  <si>
+    <t>CIK编码</t>
+  </si>
+  <si>
+    <t>fillingDate</t>
+  </si>
+  <si>
+    <t>填报日期</t>
+  </si>
+  <si>
+    <t>acceptedDate</t>
+  </si>
+  <si>
+    <t>接受日期</t>
+  </si>
+  <si>
+    <t>calendarYear</t>
+  </si>
+  <si>
+    <t>财年</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>期间</t>
+  </si>
+  <si>
+    <t>cashAndCashEquivalents</t>
+  </si>
+  <si>
+    <t>现金及现金等价物</t>
+  </si>
+  <si>
+    <t>shortTermInvestments</t>
+  </si>
+  <si>
+    <t>短期投资</t>
+  </si>
+  <si>
+    <t>cashAndShortTermInvestments</t>
+  </si>
+  <si>
+    <t>现金及短期投资总额</t>
+  </si>
+  <si>
+    <t>netReceivables</t>
+  </si>
+  <si>
+    <t>应收账款净额</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>存货</t>
+  </si>
+  <si>
+    <t>otherCurrentAssets</t>
+  </si>
+  <si>
+    <t>其他流动资产</t>
+  </si>
+  <si>
+    <t>totalCurrentAssets</t>
+  </si>
+  <si>
+    <t>流动资产总额</t>
+  </si>
+  <si>
+    <t>propertyPlantEquipmentNet</t>
+  </si>
+  <si>
+    <t>固定资产净值</t>
+  </si>
+  <si>
+    <t>goodwill</t>
+  </si>
+  <si>
+    <t>商誉</t>
+  </si>
+  <si>
+    <t>intangibleAssets</t>
+  </si>
+  <si>
+    <t>无形资产</t>
+  </si>
+  <si>
+    <t>goodwillAndIntangibleAssets</t>
+  </si>
+  <si>
+    <t>商誉和无形资产总额</t>
+  </si>
+  <si>
+    <t>longTermInvestments</t>
+  </si>
+  <si>
+    <t>长期投资</t>
+  </si>
+  <si>
+    <t>taxAssets</t>
+  </si>
+  <si>
+    <t>递延所得税资产</t>
+  </si>
+  <si>
+    <t>otherNonCurrentAssets</t>
+  </si>
+  <si>
+    <t>其他非流动资产</t>
+  </si>
+  <si>
+    <t>totalNonCurrentAssets</t>
+  </si>
+  <si>
+    <t>非流动资产总额</t>
+  </si>
+  <si>
+    <t>otherAssets</t>
+  </si>
+  <si>
+    <t>其他资产</t>
+  </si>
+  <si>
+    <t>totalAssets</t>
+  </si>
+  <si>
+    <t>总资产</t>
+  </si>
+  <si>
+    <t>accountPayables</t>
+  </si>
+  <si>
+    <t>应付账款</t>
+  </si>
+  <si>
+    <t>shortTermDebt</t>
+  </si>
+  <si>
+    <t>短期债务</t>
+  </si>
+  <si>
+    <t>taxPayables</t>
+  </si>
+  <si>
+    <t>应交税费</t>
+  </si>
+  <si>
+    <t>deferredRevenue</t>
+  </si>
+  <si>
+    <t>递延收入</t>
+  </si>
+  <si>
+    <t>otherCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>其他流动负债</t>
+  </si>
+  <si>
+    <t>totalCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>流动负债总额</t>
+  </si>
+  <si>
+    <t>longTermDebt</t>
+  </si>
+  <si>
+    <t>长期债务</t>
+  </si>
+  <si>
+    <t>deferredRevenueNonCurrent</t>
+  </si>
+  <si>
+    <t>非流动递延收入</t>
+  </si>
+  <si>
+    <t>deferredTaxLiabilitiesNonCurrent</t>
+  </si>
+  <si>
+    <t>非流动递延税负债</t>
+  </si>
+  <si>
+    <t>otherNonCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>其他非流动负债</t>
+  </si>
+  <si>
+    <t>totalNonCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>非流动负债总额</t>
+  </si>
+  <si>
+    <t>otherLiabilities</t>
+  </si>
+  <si>
+    <t>其他负债</t>
+  </si>
+  <si>
+    <t>capitalLeaseObligations</t>
+  </si>
+  <si>
+    <t>资本租赁义务</t>
+  </si>
+  <si>
+    <t>totalLiabilities</t>
+  </si>
+  <si>
+    <t>负债总额</t>
+  </si>
+  <si>
+    <t>preferredStock</t>
+  </si>
+  <si>
+    <t>优先股</t>
+  </si>
+  <si>
+    <t>commonStock</t>
+  </si>
+  <si>
+    <t>普通股</t>
+  </si>
+  <si>
+    <t>retainedEarnings</t>
+  </si>
+  <si>
+    <t>留存收益</t>
+  </si>
+  <si>
+    <t>accumulatedOtherComprehensiveIncomeLoss</t>
+  </si>
+  <si>
+    <t>累计其他综合收益/损失</t>
+  </si>
+  <si>
+    <t>othertotalStockholdersEquity</t>
+  </si>
+  <si>
+    <t>其他股东权益</t>
+  </si>
+  <si>
+    <t>totalStockholdersEquity</t>
+  </si>
+  <si>
+    <t>股东权益总额</t>
+  </si>
+  <si>
+    <t>totalEquity</t>
+  </si>
+  <si>
+    <t>总权益</t>
+  </si>
+  <si>
+    <t>totalLiabilitiesAndStockholdersEquity</t>
+  </si>
+  <si>
+    <t>负债和股东权益总额</t>
+  </si>
+  <si>
+    <t>minorityInterest</t>
+  </si>
+  <si>
+    <t>少数股东权益</t>
+  </si>
+  <si>
+    <t>totalLiabilitiesAndTotalEquity</t>
+  </si>
+  <si>
+    <t>负债和总权益总额</t>
+  </si>
+  <si>
+    <t>totalInvestments</t>
+  </si>
+  <si>
+    <t>投资总额</t>
+  </si>
+  <si>
+    <t>totalDebt</t>
+  </si>
+  <si>
+    <t>债务总额</t>
+  </si>
+  <si>
+    <t>netDebt</t>
+  </si>
+  <si>
+    <t>净债务</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>链接</t>
+  </si>
+  <si>
+    <t>finalLink</t>
+  </si>
+  <si>
+    <t>最终链接</t>
+  </si>
+  <si>
+    <t>如果需要导出为Excel或CSV格式，请告诉我，我可以帮助生成文件内容。</t>
+  </si>
+  <si>
+    <t>fmp</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>filing_date</t>
+  </si>
+  <si>
+    <t>accepted_date</t>
+  </si>
+  <si>
+    <t>reported_currency</t>
+  </si>
+  <si>
+    <t>cash_and_cash_equivalents</t>
+  </si>
+  <si>
+    <t>short_term_investments</t>
+  </si>
+  <si>
+    <t>cash_and_short_term_investments</t>
+  </si>
+  <si>
+    <t>net_receivables</t>
+  </si>
+  <si>
+    <t>inventories</t>
+  </si>
+  <si>
+    <t>other_current_assets</t>
+  </si>
+  <si>
+    <t>total_current_assets</t>
+  </si>
+  <si>
+    <t>plant_property_equipment_net</t>
+  </si>
+  <si>
+    <t>intangible_assets</t>
+  </si>
+  <si>
+    <t>goodwill_and_intangible_assets</t>
+  </si>
+  <si>
+    <t>long_term_investments</t>
+  </si>
+  <si>
+    <t>tax_assets</t>
+  </si>
+  <si>
+    <t>other_non_current_assets</t>
+  </si>
+  <si>
+    <t>non_current_assets</t>
+  </si>
+  <si>
+    <t>other_assets</t>
+  </si>
+  <si>
+    <t>total_assets</t>
+  </si>
+  <si>
+    <t>accounts_payable</t>
+  </si>
+  <si>
+    <t>short_term_debt</t>
+  </si>
+  <si>
+    <t>tax_payables</t>
+  </si>
+  <si>
+    <t>current_deferred_revenue</t>
+  </si>
+  <si>
+    <t>other_current_liabilities</t>
+  </si>
+  <si>
+    <t>total_current_liabilities</t>
+  </si>
+  <si>
+    <t>long_term_debt</t>
+  </si>
+  <si>
+    <t>deferred_revenue_non_current</t>
+  </si>
+  <si>
+    <t>deferred_tax_liabilities_non_current</t>
+  </si>
+  <si>
+    <t>other_non_current_liabilities</t>
+  </si>
+  <si>
+    <t>total_non_current_liabilities</t>
+  </si>
+  <si>
+    <t>other_liabilities</t>
+  </si>
+  <si>
+    <t>capital_lease_obligations</t>
+  </si>
+  <si>
+    <t>total_liabilities</t>
+  </si>
+  <si>
+    <t>preferred_stock</t>
+  </si>
+  <si>
+    <t>common_stock</t>
+  </si>
+  <si>
+    <t>retained_earnings</t>
+  </si>
+  <si>
+    <t>accumulated_other_comprehensive_income</t>
+  </si>
+  <si>
+    <t>other_shareholders_equity</t>
+  </si>
+  <si>
+    <t>otherStockholdersEquity</t>
+  </si>
+  <si>
+    <t>other_total_shareholders_equity</t>
+  </si>
+  <si>
+    <t>total_common_equity</t>
+  </si>
+  <si>
+    <t>total_equity_non_controlling_interests</t>
+  </si>
+  <si>
+    <t>total_liabilities_and_shareholders_equity</t>
+  </si>
+  <si>
+    <t>minority_interest</t>
+  </si>
+  <si>
+    <t>total_liabilities_and_total_equity</t>
+  </si>
+  <si>
+    <t>total_investments</t>
+  </si>
+  <si>
+    <t>total_debt</t>
+  </si>
+  <si>
+    <t>net_debt</t>
+  </si>
+  <si>
+    <t>final_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -313,7 +711,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -343,6 +741,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -352,7 +765,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -375,30 +788,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -406,14 +816,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -451,7 +864,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -523,7 +936,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -696,22 +1109,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.52734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -739,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -754,26 +1167,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.64453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -787,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -801,7 +1215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -815,7 +1229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -823,7 +1237,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -833,7 +1247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -841,7 +1255,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -849,7 +1263,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -858,6 +1272,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -865,70 +1280,1252 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="1" max="1" width="43.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" customWidth="1"/>
+    <col min="6" max="6" width="22.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A35" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A45" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A46" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A47" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A48" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A49" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A50" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A51" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A52" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A53" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A54" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="6" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B60123B-785D-4CD3-AB4D-AF48E9FF3083}">
+  <dimension ref="A1:B59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="23.3515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A33" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A36" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A38" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A43" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A45" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="71.7" x14ac:dyDescent="0.4">
+      <c r="A46" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A47" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+      <c r="A48" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A49" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="71.7" x14ac:dyDescent="0.4">
+      <c r="A50" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A51" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+      <c r="A52" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A53" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A54" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+      <c r="A57" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Supported balance sheet for A-Share
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF31B926-A3F4-48C5-AB17-03C015CB9D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="11472"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -23,12 +17,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="204">
   <si>
     <t>Model</t>
   </si>
@@ -693,17 +687,53 @@
   </si>
   <si>
     <t>final_link</t>
+  </si>
+  <si>
+    <t>A股</t>
+  </si>
+  <si>
+    <t>港股</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>EquityQuoteData</t>
+  </si>
+  <si>
+    <t>AKShareEquityQuoteData</t>
+  </si>
+  <si>
+    <t>EquityHistoricalData</t>
+  </si>
+  <si>
+    <t>AKShareEquityHistoricalData</t>
+  </si>
+  <si>
+    <t>AKShareHistoricalDividendsData</t>
+  </si>
+  <si>
+    <t>HistoricalDividendsData</t>
+  </si>
+  <si>
+    <t>AKShare did not support all HKEX data.</t>
+  </si>
+  <si>
+    <t>CompanyNewsData</t>
+  </si>
+  <si>
+    <t>AKShareCompanyNewsData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -711,7 +741,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -745,13 +775,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -808,7 +838,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -824,9 +854,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -864,7 +894,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -936,7 +966,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1109,61 +1139,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.52734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="D1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1174,20 +1277,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="19.64453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1215,7 +1318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1229,7 +1332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -1237,7 +1340,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -1247,7 +1350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -1255,7 +1358,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1263,7 +1366,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1280,27 +1383,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.64453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.87890625" customWidth="1"/>
-    <col min="6" max="6" width="22.05859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1320,7 +1423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1336,7 +1439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1352,7 +1455,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1368,7 +1471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>143</v>
       </c>
@@ -1382,7 +1485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>144</v>
       </c>
@@ -1396,7 +1499,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>145</v>
       </c>
@@ -1410,7 +1513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>146</v>
       </c>
@@ -1424,7 +1527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>147</v>
       </c>
@@ -1438,7 +1541,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>148</v>
       </c>
@@ -1452,7 +1555,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
         <v>149</v>
       </c>
@@ -1466,7 +1569,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
         <v>150</v>
       </c>
@@ -1480,7 +1583,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
         <v>151</v>
       </c>
@@ -1494,7 +1597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
         <v>152</v>
       </c>
@@ -1508,7 +1611,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
         <v>153</v>
       </c>
@@ -1522,7 +1625,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
         <v>154</v>
       </c>
@@ -1536,7 +1639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>155</v>
       </c>
@@ -1550,7 +1653,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>156</v>
       </c>
@@ -1564,7 +1667,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
         <v>157</v>
       </c>
@@ -1578,7 +1681,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
         <v>158</v>
       </c>
@@ -1592,7 +1695,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>159</v>
       </c>
@@ -1606,7 +1709,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6">
       <c r="A23" s="6" t="s">
         <v>160</v>
       </c>
@@ -1620,7 +1723,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6">
       <c r="A24" s="6" t="s">
         <v>161</v>
       </c>
@@ -1634,7 +1737,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
         <v>162</v>
       </c>
@@ -1648,7 +1751,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6">
       <c r="A26" s="6" t="s">
         <v>163</v>
       </c>
@@ -1662,7 +1765,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6">
       <c r="A27" s="6" t="s">
         <v>164</v>
       </c>
@@ -1676,7 +1779,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6">
       <c r="A28" s="6" t="s">
         <v>165</v>
       </c>
@@ -1690,7 +1793,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
         <v>166</v>
       </c>
@@ -1704,7 +1807,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
         <v>167</v>
       </c>
@@ -1718,7 +1821,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
         <v>168</v>
       </c>
@@ -1732,7 +1835,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
         <v>169</v>
       </c>
@@ -1746,7 +1849,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
         <v>170</v>
       </c>
@@ -1760,7 +1863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6">
       <c r="A34" s="6" t="s">
         <v>171</v>
       </c>
@@ -1774,7 +1877,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6">
       <c r="A35" s="6" t="s">
         <v>172</v>
       </c>
@@ -1788,7 +1891,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6">
       <c r="A36" s="6" t="s">
         <v>173</v>
       </c>
@@ -1802,7 +1905,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6">
       <c r="A37" s="6" t="s">
         <v>174</v>
       </c>
@@ -1816,7 +1919,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6">
       <c r="A38" s="6" t="s">
         <v>175</v>
       </c>
@@ -1830,7 +1933,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6">
       <c r="A39" s="6" t="s">
         <v>176</v>
       </c>
@@ -1844,7 +1947,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6">
       <c r="A40" s="6" t="s">
         <v>177</v>
       </c>
@@ -1858,7 +1961,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6">
       <c r="A41" s="6" t="s">
         <v>178</v>
       </c>
@@ -1872,7 +1975,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6">
       <c r="A42" s="6" t="s">
         <v>179</v>
       </c>
@@ -1886,7 +1989,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6">
       <c r="A43" s="6" t="s">
         <v>180</v>
       </c>
@@ -1900,7 +2003,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6">
       <c r="A44" s="6" t="s">
         <v>182</v>
       </c>
@@ -1914,7 +2017,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6">
       <c r="A45" s="6" t="s">
         <v>183</v>
       </c>
@@ -1928,7 +2031,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6">
       <c r="A46" s="6" t="s">
         <v>184</v>
       </c>
@@ -1942,7 +2045,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6">
       <c r="A47" s="6" t="s">
         <v>185</v>
       </c>
@@ -1956,7 +2059,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6">
       <c r="A48" s="6" t="s">
         <v>186</v>
       </c>
@@ -1970,7 +2073,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6">
       <c r="A49" s="6" t="s">
         <v>187</v>
       </c>
@@ -1984,7 +2087,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6">
       <c r="A50" s="6" t="s">
         <v>188</v>
       </c>
@@ -1998,7 +2101,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6">
       <c r="A51" s="6" t="s">
         <v>189</v>
       </c>
@@ -2012,7 +2115,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6">
       <c r="A52" s="6" t="s">
         <v>190</v>
       </c>
@@ -2026,7 +2129,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6">
       <c r="A53" s="6" t="s">
         <v>137</v>
       </c>
@@ -2040,7 +2143,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6">
       <c r="A54" s="6" t="s">
         <v>191</v>
       </c>
@@ -2061,24 +2164,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B60123B-785D-4CD3-AB4D-AF48E9FF3083}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="23.3515625" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2086,7 +2189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -2094,7 +2197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -2102,7 +2205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -2110,7 +2213,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2118,7 +2221,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -2126,7 +2229,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
@@ -2134,7 +2237,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>45</v>
       </c>
@@ -2142,7 +2245,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
@@ -2150,7 +2253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
@@ -2158,7 +2261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -2166,7 +2269,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="28.8">
       <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
@@ -2174,7 +2277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
         <v>55</v>
       </c>
@@ -2182,7 +2285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>57</v>
       </c>
@@ -2190,7 +2293,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>59</v>
       </c>
@@ -2198,7 +2301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>61</v>
       </c>
@@ -2206,7 +2309,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="28.8">
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
@@ -2214,7 +2317,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>65</v>
       </c>
@@ -2222,7 +2325,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>67</v>
       </c>
@@ -2230,7 +2333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="28.8">
       <c r="A22" s="5" t="s">
         <v>69</v>
       </c>
@@ -2238,7 +2341,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>71</v>
       </c>
@@ -2246,7 +2349,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
         <v>73</v>
       </c>
@@ -2254,7 +2357,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2">
       <c r="A25" s="5" t="s">
         <v>75</v>
       </c>
@@ -2262,7 +2365,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
         <v>77</v>
       </c>
@@ -2270,7 +2373,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
         <v>79</v>
       </c>
@@ -2278,7 +2381,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
         <v>81</v>
       </c>
@@ -2286,7 +2389,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2">
       <c r="A29" s="5" t="s">
         <v>83</v>
       </c>
@@ -2294,7 +2397,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>85</v>
       </c>
@@ -2302,7 +2405,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
         <v>87</v>
       </c>
@@ -2310,7 +2413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
@@ -2318,7 +2421,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>91</v>
       </c>
@@ -2326,7 +2429,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -2334,7 +2437,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
         <v>95</v>
       </c>
@@ -2342,7 +2445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" ht="28.8">
       <c r="A36" s="5" t="s">
         <v>97</v>
       </c>
@@ -2350,7 +2453,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" ht="28.8">
       <c r="A37" s="5" t="s">
         <v>99</v>
       </c>
@@ -2358,7 +2461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2">
       <c r="A38" s="5" t="s">
         <v>101</v>
       </c>
@@ -2366,7 +2469,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2">
       <c r="A39" s="5" t="s">
         <v>103</v>
       </c>
@@ -2374,7 +2477,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2">
       <c r="A40" s="5" t="s">
         <v>105</v>
       </c>
@@ -2382,7 +2485,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2">
       <c r="A41" s="5" t="s">
         <v>107</v>
       </c>
@@ -2390,7 +2493,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2">
       <c r="A42" s="5" t="s">
         <v>109</v>
       </c>
@@ -2398,7 +2501,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2">
       <c r="A43" s="5" t="s">
         <v>111</v>
       </c>
@@ -2406,7 +2509,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2">
       <c r="A44" s="5" t="s">
         <v>113</v>
       </c>
@@ -2414,7 +2517,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2">
       <c r="A45" s="5" t="s">
         <v>115</v>
       </c>
@@ -2422,7 +2525,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="71.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" ht="28.8">
       <c r="A46" s="5" t="s">
         <v>117</v>
       </c>
@@ -2430,7 +2533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" ht="28.8">
       <c r="A47" s="5" t="s">
         <v>119</v>
       </c>
@@ -2438,7 +2541,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="43" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2">
       <c r="A48" s="5" t="s">
         <v>121</v>
       </c>
@@ -2446,7 +2549,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:2">
       <c r="A49" s="5" t="s">
         <v>123</v>
       </c>
@@ -2454,7 +2557,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="71.7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:2" ht="28.8">
       <c r="A50" s="5" t="s">
         <v>125</v>
       </c>
@@ -2462,7 +2565,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:2">
       <c r="A51" s="5" t="s">
         <v>127</v>
       </c>
@@ -2470,7 +2573,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="57.35" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:2" ht="28.8">
       <c r="A52" s="5" t="s">
         <v>129</v>
       </c>
@@ -2478,7 +2581,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:2">
       <c r="A53" s="5" t="s">
         <v>131</v>
       </c>
@@ -2486,7 +2589,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:2">
       <c r="A54" s="5" t="s">
         <v>133</v>
       </c>
@@ -2494,7 +2597,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:2">
       <c r="A55" s="5" t="s">
         <v>135</v>
       </c>
@@ -2502,7 +2605,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:2">
       <c r="A56" s="5" t="s">
         <v>137</v>
       </c>
@@ -2510,7 +2613,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="28.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:2">
       <c r="A57" s="5" t="s">
         <v>139</v>
       </c>
@@ -2518,7 +2621,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
Added Cash Flow model
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -1,28 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05071CF8-5FA4-4D14-B0C3-5435268A3687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13512" yWindow="132" windowWidth="15060" windowHeight="11472" activeTab="3"/>
+    <workbookView xWindow="4400" yWindow="207" windowWidth="14700" windowHeight="10973" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="AvailableIndices" sheetId="2" r:id="rId2"/>
-    <sheet name="BalanceSheetData" sheetId="3" r:id="rId3"/>
-    <sheet name="IncomeStatementData" sheetId="4" r:id="rId4"/>
+    <sheet name="BalanceSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="IncomeStatement" sheetId="4" r:id="rId4"/>
+    <sheet name="CashFlowStatement" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="403">
   <si>
     <t>Model</t>
   </si>
@@ -971,12 +978,6 @@
     <t>​​字段名 (原始键)​​</t>
   </si>
   <si>
-    <t>​​API字段名​​</t>
-  </si>
-  <si>
-    <t>​​中文翻译​​</t>
-  </si>
-  <si>
     <t>EBITDA利润率</t>
   </si>
   <si>
@@ -1011,17 +1012,344 @@
   </si>
   <si>
     <t>DILUTED_EPS</t>
+  </si>
+  <si>
+    <t>AKShareIncomeStatementData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CashFlowStatementData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>FMPCashFlowStatementData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>YFinanceCashFlowStatementData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>AKShareCashFlowStatementData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>东财</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>FMP</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>​​FMP(中文)​​</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>net_income</t>
+  </si>
+  <si>
+    <t>净利润</t>
+  </si>
+  <si>
+    <t>deferred_income_tax</t>
+  </si>
+  <si>
+    <t>deferredIncomeTax</t>
+  </si>
+  <si>
+    <t>递延所得税</t>
+  </si>
+  <si>
+    <t>stock_based_compensation</t>
+  </si>
+  <si>
+    <t>stockBasedCompensation</t>
+  </si>
+  <si>
+    <t>股权激励费用</t>
+  </si>
+  <si>
+    <t>change_in_working_capital</t>
+  </si>
+  <si>
+    <t>changeInWorkingCapital</t>
+  </si>
+  <si>
+    <t>营运资本变动总额</t>
+  </si>
+  <si>
+    <t>change_in_account_receivables</t>
+  </si>
+  <si>
+    <t>accountsReceivables</t>
+  </si>
+  <si>
+    <t>应收账款变动</t>
+  </si>
+  <si>
+    <t>change_in_inventory</t>
+  </si>
+  <si>
+    <t>存货变动</t>
+  </si>
+  <si>
+    <t>change_in_account_payable</t>
+  </si>
+  <si>
+    <t>accountsPayables</t>
+  </si>
+  <si>
+    <t>应付账款变动</t>
+  </si>
+  <si>
+    <t>change_in_other_working_capital</t>
+  </si>
+  <si>
+    <t>otherWorkingCapital</t>
+  </si>
+  <si>
+    <t>其他营运资本变动</t>
+  </si>
+  <si>
+    <t>change_in_other_non_cash_items</t>
+  </si>
+  <si>
+    <t>otherNonCashItems</t>
+  </si>
+  <si>
+    <t>其他非现金项目变动</t>
+  </si>
+  <si>
+    <t>net_cash_from_operating_activities</t>
+  </si>
+  <si>
+    <t>netCashProvidedByOperatingActivities</t>
+  </si>
+  <si>
+    <t>经营活动现金流量净额</t>
+  </si>
+  <si>
+    <t>purchase_of_property_plant_and_equipment</t>
+  </si>
+  <si>
+    <t>investmentsInPropertyPlantAndEquipment</t>
+  </si>
+  <si>
+    <t>不动产/厂房/设备购置</t>
+  </si>
+  <si>
+    <t>acquisitions</t>
+  </si>
+  <si>
+    <t>acquisitionsNet</t>
+  </si>
+  <si>
+    <t>收购活动净额</t>
+  </si>
+  <si>
+    <t>purchase_of_investment_securities</t>
+  </si>
+  <si>
+    <t>purchasesOfInvestments</t>
+  </si>
+  <si>
+    <t>购买投资证券</t>
+  </si>
+  <si>
+    <t>sale_and_maturity_of_investments</t>
+  </si>
+  <si>
+    <t>salesMaturitiesOfInvestments</t>
+  </si>
+  <si>
+    <t>出售及到期投资</t>
+  </si>
+  <si>
+    <t>other_investing_activities</t>
+  </si>
+  <si>
+    <t>otherInvestingActivites</t>
+  </si>
+  <si>
+    <t>其他投资活动</t>
+  </si>
+  <si>
+    <t>net_cash_from_investing_activities</t>
+  </si>
+  <si>
+    <t>netCashUsedForInvestingActivites</t>
+  </si>
+  <si>
+    <t>投资活动现金流量净额</t>
+  </si>
+  <si>
+    <t>repayment_of_debt</t>
+  </si>
+  <si>
+    <t>debtRepayment</t>
+  </si>
+  <si>
+    <t>债务偿还</t>
+  </si>
+  <si>
+    <t>issuance_of_common_equity</t>
+  </si>
+  <si>
+    <t>commonStockIssued</t>
+  </si>
+  <si>
+    <t>发行普通股</t>
+  </si>
+  <si>
+    <t>repurchase_of_common_equity</t>
+  </si>
+  <si>
+    <t>commonStockRepurchased</t>
+  </si>
+  <si>
+    <t>回购普通股</t>
+  </si>
+  <si>
+    <t>payment_of_dividends</t>
+  </si>
+  <si>
+    <t>dividendsPaid</t>
+  </si>
+  <si>
+    <t>支付股息</t>
+  </si>
+  <si>
+    <t>other_financing_activities</t>
+  </si>
+  <si>
+    <t>otherFinancingActivites</t>
+  </si>
+  <si>
+    <t>其他筹资活动</t>
+  </si>
+  <si>
+    <t>net_cash_from_financing_activities</t>
+  </si>
+  <si>
+    <t>netCashUsedProvidedByFinancingActivities</t>
+  </si>
+  <si>
+    <t>筹资活动现金流量净额</t>
+  </si>
+  <si>
+    <t>effect_of_exchange_rate_changes_on_cash</t>
+  </si>
+  <si>
+    <t>effectOfForexChangesOnCash</t>
+  </si>
+  <si>
+    <t>汇率变动对现金的影响</t>
+  </si>
+  <si>
+    <t>net_change_in_cash_and_equivalents</t>
+  </si>
+  <si>
+    <t>netChangeInCash</t>
+  </si>
+  <si>
+    <t>现金及等价物净变动额</t>
+  </si>
+  <si>
+    <t>cash_at_beginning_of_period</t>
+  </si>
+  <si>
+    <t>cashAtBeginningOfPeriod</t>
+  </si>
+  <si>
+    <t>期初现金余额</t>
+  </si>
+  <si>
+    <t>cash_at_end_of_period</t>
+  </si>
+  <si>
+    <t>cashAtEndOfPeriod</t>
+  </si>
+  <si>
+    <t>期末现金余额</t>
+  </si>
+  <si>
+    <t>operating_cash_flow</t>
+  </si>
+  <si>
+    <t>operatingCashFlow</t>
+  </si>
+  <si>
+    <t>经营活动现金流量(简)</t>
+  </si>
+  <si>
+    <t>capital_expenditure</t>
+  </si>
+  <si>
+    <t>capitalExpenditure</t>
+  </si>
+  <si>
+    <t>资本支出</t>
+  </si>
+  <si>
+    <t>free_cash_flow</t>
+  </si>
+  <si>
+    <t>freeCashFlow</t>
+  </si>
+  <si>
+    <t>自由现金流</t>
+  </si>
+  <si>
+    <t>SEC文件索引链接</t>
+  </si>
+  <si>
+    <t>​​Original Key​​</t>
+  </si>
+  <si>
+    <t>​​经营活动现金流​​</t>
+  </si>
+  <si>
+    <t>​​投资活动现金流​​</t>
+  </si>
+  <si>
+    <t>​​筹资活动现金流​​</t>
+  </si>
+  <si>
+    <t>​​现金变动与校验​​</t>
+  </si>
+  <si>
+    <t>​​衍生指标​​</t>
+  </si>
+  <si>
+    <t>​​数据源​​</t>
+  </si>
+  <si>
+    <t>REPORT_DATE</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>REPORT_TYPE</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CURRENCY</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1029,7 +1357,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1061,7 +1389,16 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1075,7 +1412,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1098,11 +1435,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1110,9 +1458,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1128,9 +1479,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1168,7 +1519,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1240,7 +1591,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1413,27 +1764,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="D1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1804,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1471,7 +1822,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1489,7 +1840,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -1501,7 +1852,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -1515,7 +1866,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -1529,7 +1880,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -1543,7 +1894,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>195</v>
       </c>
@@ -1552,6 +1903,27 @@
       </c>
       <c r="C9" t="s">
         <v>196</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -1562,20 +1934,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.64453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +1961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1603,7 +1975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1617,7 +1989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -1625,7 +1997,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -1635,7 +2007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -1643,7 +2015,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1651,7 +2023,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1668,27 +2040,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" customWidth="1"/>
+    <col min="6" max="6" width="22.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1708,7 +2080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1724,7 +2096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1740,7 +2112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1756,7 +2128,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>134</v>
       </c>
@@ -1770,7 +2142,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>135</v>
       </c>
@@ -1784,7 +2156,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>136</v>
       </c>
@@ -1798,7 +2170,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>137</v>
       </c>
@@ -1812,7 +2184,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>138</v>
       </c>
@@ -1826,7 +2198,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>139</v>
       </c>
@@ -1840,7 +2212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>140</v>
       </c>
@@ -1854,7 +2226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
@@ -1868,7 +2240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>142</v>
       </c>
@@ -1882,7 +2254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>143</v>
       </c>
@@ -1896,7 +2268,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>144</v>
       </c>
@@ -1910,7 +2282,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>145</v>
       </c>
@@ -1924,7 +2296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>146</v>
       </c>
@@ -1938,7 +2310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>147</v>
       </c>
@@ -1952,7 +2324,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>148</v>
       </c>
@@ -1966,7 +2338,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>149</v>
       </c>
@@ -1980,7 +2352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>150</v>
       </c>
@@ -1994,7 +2366,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -2008,7 +2380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -2022,7 +2394,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>153</v>
       </c>
@@ -2036,7 +2408,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>154</v>
       </c>
@@ -2050,7 +2422,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -2064,7 +2436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -2078,7 +2450,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>157</v>
       </c>
@@ -2092,7 +2464,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>158</v>
       </c>
@@ -2106,7 +2478,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>159</v>
       </c>
@@ -2120,7 +2492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>160</v>
       </c>
@@ -2134,7 +2506,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -2148,7 +2520,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>162</v>
       </c>
@@ -2162,7 +2534,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>163</v>
       </c>
@@ -2176,7 +2548,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>164</v>
       </c>
@@ -2190,7 +2562,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>165</v>
       </c>
@@ -2204,7 +2576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>166</v>
       </c>
@@ -2218,7 +2590,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>167</v>
       </c>
@@ -2232,7 +2604,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>168</v>
       </c>
@@ -2246,7 +2618,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>169</v>
       </c>
@@ -2260,7 +2632,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>170</v>
       </c>
@@ -2274,7 +2646,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>171</v>
       </c>
@@ -2288,7 +2660,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>173</v>
       </c>
@@ -2302,7 +2674,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>174</v>
       </c>
@@ -2316,7 +2688,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>175</v>
       </c>
@@ -2330,7 +2702,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
         <v>176</v>
       </c>
@@ -2344,7 +2716,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>177</v>
       </c>
@@ -2358,7 +2730,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>178</v>
       </c>
@@ -2372,7 +2744,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>179</v>
       </c>
@@ -2386,7 +2758,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>180</v>
       </c>
@@ -2400,7 +2772,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>181</v>
       </c>
@@ -2414,7 +2786,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>129</v>
       </c>
@@ -2428,7 +2800,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -2449,461 +2821,1035 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.234375" customWidth="1"/>
+    <col min="2" max="2" width="28.41015625" customWidth="1"/>
+    <col min="3" max="3" width="19.234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>214</v>
-      </c>
-      <c r="B13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C13" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" t="s">
-        <v>221</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>223</v>
-      </c>
-      <c r="B16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>226</v>
-      </c>
-      <c r="B17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>229</v>
-      </c>
-      <c r="B18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>232</v>
-      </c>
-      <c r="B19" t="s">
-        <v>233</v>
-      </c>
-      <c r="C19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B20" t="s">
-        <v>236</v>
-      </c>
-      <c r="C20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B22" t="s">
-        <v>242</v>
-      </c>
-      <c r="C22" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>244</v>
-      </c>
-      <c r="B23" t="s">
-        <v>244</v>
-      </c>
-      <c r="C23" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>246</v>
-      </c>
-      <c r="B24" t="s">
-        <v>247</v>
-      </c>
-      <c r="C24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>248</v>
-      </c>
-      <c r="B25" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" t="s">
-        <v>250</v>
-      </c>
-      <c r="D25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>251</v>
-      </c>
-      <c r="B26" t="s">
-        <v>252</v>
-      </c>
-      <c r="C26" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>254</v>
-      </c>
-      <c r="B27" t="s">
-        <v>255</v>
-      </c>
-      <c r="C27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>257</v>
-      </c>
-      <c r="B28" t="s">
-        <v>258</v>
-      </c>
-      <c r="C28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D28" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>260</v>
-      </c>
-      <c r="B29" t="s">
-        <v>261</v>
-      </c>
-      <c r="C29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>263</v>
-      </c>
-      <c r="B30" t="s">
-        <v>264</v>
-      </c>
-      <c r="C30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D30" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>266</v>
-      </c>
-      <c r="B31" t="s">
-        <v>267</v>
-      </c>
-      <c r="C31" t="s">
-        <v>268</v>
-      </c>
-      <c r="D31" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>269</v>
-      </c>
-      <c r="B32" t="s">
-        <v>270</v>
-      </c>
-      <c r="C32" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>272</v>
-      </c>
-      <c r="B33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C33" t="s">
-        <v>274</v>
-      </c>
-      <c r="D33" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>275</v>
-      </c>
-      <c r="B34" t="s">
-        <v>276</v>
-      </c>
-      <c r="C34" t="s">
-        <v>277</v>
-      </c>
-      <c r="D34" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>278</v>
-      </c>
-      <c r="B35" t="s">
-        <v>279</v>
-      </c>
-      <c r="C35" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>281</v>
-      </c>
-      <c r="B36" t="s">
-        <v>282</v>
-      </c>
-      <c r="C36" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>284</v>
       </c>
+      <c r="D38" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A34D0A0-C4C1-401F-9DA9-80D98685DB3F}">
+  <dimension ref="A2:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="42.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.17578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on currency_historical and currency_snapshots
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="204" windowWidth="14700" windowHeight="10968" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="4404" yWindow="204" windowWidth="14700" windowHeight="10968" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="BalanceSheet" sheetId="3" r:id="rId3"/>
     <sheet name="IncomeStatement" sheetId="4" r:id="rId4"/>
     <sheet name="CashFlowStatement" sheetId="5" r:id="rId5"/>
+    <sheet name="CurrencyHistorical" sheetId="6" r:id="rId6"/>
+    <sheet name="CurrencySnapshots" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -111,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="429">
   <si>
     <t>Model</t>
   </si>
@@ -1325,6 +1327,90 @@
   <si>
     <t>REPORT_DATE</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurrencyHistoricalData</t>
+  </si>
+  <si>
+    <t>FMPCurrencySnapshotsData</t>
+  </si>
+  <si>
+    <t>YFinanceCurrencyHistoricalData</t>
+  </si>
+  <si>
+    <t>CurrencySnapshotsData</t>
+  </si>
+  <si>
+    <t>AKShareCurrencySnapshotsData</t>
+  </si>
+  <si>
+    <t>AKShareCurrencyHistoricalData</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>vwap</t>
+  </si>
+  <si>
+    <t>今开</t>
+  </si>
+  <si>
+    <t>最高</t>
+  </si>
+  <si>
+    <t>最低</t>
+  </si>
+  <si>
+    <t>base_currency</t>
+  </si>
+  <si>
+    <t>counter_currency</t>
+  </si>
+  <si>
+    <t>prev_close</t>
+  </si>
+  <si>
+    <t>昨收</t>
+  </si>
+  <si>
+    <t>代码</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>最新价</t>
+  </si>
+  <si>
+    <t>涨跌额</t>
+  </si>
+  <si>
+    <t>涨跌幅</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>change_percent</t>
+  </si>
+  <si>
+    <t>last_rate</t>
+  </si>
+  <si>
+    <t>振幅</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1484,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1421,17 +1507,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1444,9 +1519,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1751,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1828,10 +1905,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>194</v>
+        <v>300</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>185</v>
@@ -1840,77 +1923,101 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>185</v>
-      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="B7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C7" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>404</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>300</v>
-      </c>
-      <c r="B10" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" t="s">
-        <v>301</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>303</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2823,16 +2930,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3299,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3311,16 +3418,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3403,7 +3510,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>394</v>
       </c>
       <c r="B9" s="3"/>
@@ -3543,7 +3650,7 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>395</v>
       </c>
       <c r="B21" s="3"/>
@@ -3623,7 +3730,7 @@
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>396</v>
       </c>
       <c r="B28" s="3"/>
@@ -3839,4 +3946,361 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added HK in equity_quote.py
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10021C3D-93A1-4900-B207-341E705B83F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="207" windowWidth="12960" windowHeight="10973" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6144" yWindow="204" windowWidth="12960" windowHeight="10968" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -27,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="474">
   <si>
     <t>Model</t>
   </si>
@@ -1591,17 +1585,23 @@
   <si>
     <t>昨收</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>东财(A)</t>
+  </si>
+  <si>
+    <t>东财(HK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1609,7 +1609,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1641,7 +1641,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1650,7 +1650,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1691,7 +1691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1703,13 +1703,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1725,9 +1724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1765,7 +1764,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1837,7 +1836,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2010,27 +2009,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.64453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.87890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="D1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2049,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2068,7 +2067,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2086,7 +2085,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -2104,7 +2103,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -2116,7 +2115,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>400</v>
       </c>
@@ -2132,7 +2131,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>403</v>
       </c>
@@ -2142,7 +2141,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>428</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>194</v>
       </c>
@@ -2210,20 +2209,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="19.64453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2237,7 +2236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -2273,7 +2272,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -2283,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -2291,7 +2290,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -2299,7 +2298,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2316,27 +2315,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.64453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.87890625" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +2355,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -2372,7 +2371,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>134</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>135</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>136</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>137</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>138</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>139</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>140</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>142</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>143</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>144</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>145</v>
       </c>
@@ -2572,7 +2571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>146</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>147</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>148</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>149</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>150</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>153</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>154</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
         <v>157</v>
       </c>
@@ -2740,7 +2739,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>158</v>
       </c>
@@ -2754,7 +2753,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>159</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>160</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>162</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>163</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>164</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>165</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>166</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>167</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>168</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>169</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>170</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>171</v>
       </c>
@@ -2936,7 +2935,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>173</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>174</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>175</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>176</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
         <v>177</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
         <v>178</v>
       </c>
@@ -3020,7 +3019,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
         <v>179</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
         <v>180</v>
       </c>
@@ -3048,7 +3047,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>181</v>
       </c>
@@ -3062,7 +3061,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
         <v>129</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -3097,21 +3096,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="42.64453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -3165,7 +3164,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
@@ -3177,7 +3176,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
@@ -3189,7 +3188,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
@@ -3203,7 +3202,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
         <v>393</v>
       </c>
@@ -3211,7 +3210,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>306</v>
       </c>
@@ -3223,7 +3222,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>240</v>
       </c>
@@ -3235,7 +3234,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>308</v>
       </c>
@@ -3247,7 +3246,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>311</v>
       </c>
@@ -3259,7 +3258,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>314</v>
       </c>
@@ -3271,7 +3270,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>317</v>
       </c>
@@ -3283,7 +3282,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>320</v>
       </c>
@@ -3295,7 +3294,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>322</v>
       </c>
@@ -3307,7 +3306,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>325</v>
       </c>
@@ -3319,7 +3318,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>328</v>
       </c>
@@ -3331,7 +3330,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>331</v>
       </c>
@@ -3343,7 +3342,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
         <v>394</v>
       </c>
@@ -3351,7 +3350,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
         <v>334</v>
       </c>
@@ -3363,7 +3362,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>337</v>
       </c>
@@ -3375,7 +3374,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>340</v>
       </c>
@@ -3387,7 +3386,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>343</v>
       </c>
@@ -3399,7 +3398,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>346</v>
       </c>
@@ -3411,7 +3410,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>349</v>
       </c>
@@ -3423,7 +3422,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
         <v>395</v>
       </c>
@@ -3431,7 +3430,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
         <v>352</v>
       </c>
@@ -3443,7 +3442,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>355</v>
       </c>
@@ -3455,7 +3454,7 @@
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>358</v>
       </c>
@@ -3467,7 +3466,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>361</v>
       </c>
@@ -3479,7 +3478,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>364</v>
       </c>
@@ -3491,7 +3490,7 @@
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>367</v>
       </c>
@@ -3503,7 +3502,7 @@
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>396</v>
       </c>
@@ -3511,7 +3510,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>370</v>
       </c>
@@ -3523,7 +3522,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
         <v>373</v>
       </c>
@@ -3535,7 +3534,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
         <v>376</v>
       </c>
@@ -3547,7 +3546,7 @@
       </c>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
         <v>379</v>
       </c>
@@ -3559,7 +3558,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>397</v>
       </c>
@@ -3567,7 +3566,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
         <v>382</v>
       </c>
@@ -3579,7 +3578,7 @@
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
         <v>385</v>
       </c>
@@ -3591,7 +3590,7 @@
       </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>388</v>
       </c>
@@ -3603,7 +3602,7 @@
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>398</v>
       </c>
@@ -3611,7 +3610,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>129</v>
       </c>
@@ -3623,7 +3622,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>182</v>
       </c>
@@ -3643,23 +3642,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="4.76171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -3676,7 +3675,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>406</v>
       </c>
@@ -3702,7 +3701,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>407</v>
       </c>
@@ -3715,7 +3714,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>408</v>
       </c>
@@ -3728,7 +3727,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>409</v>
       </c>
@@ -3739,7 +3738,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>410</v>
       </c>
@@ -3750,7 +3749,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>411</v>
       </c>
@@ -3761,7 +3760,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -3772,7 +3771,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>426</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>424</v>
       </c>
@@ -3812,20 +3811,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -3842,7 +3841,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>415</v>
       </c>
@@ -3853,7 +3852,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>416</v>
       </c>
@@ -3864,7 +3863,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>426</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>406</v>
       </c>
@@ -3890,7 +3889,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>407</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>408</v>
       </c>
@@ -3916,7 +3915,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>409</v>
       </c>
@@ -3927,7 +3926,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>410</v>
       </c>
@@ -3938,7 +3937,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>417</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3962,7 +3961,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="15.6" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6" t="s">
@@ -3984,7 +3983,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -4002,23 +4001,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527DE59B-D1AB-406C-BD26-669AE9370541}">
-  <dimension ref="A2:E35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.52734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -4032,302 +4031,447 @@
         <v>305</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="F5" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="F21" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E25" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="F25" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E26" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+      <c r="F26" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E27" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+      <c r="F27" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E29" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="F29" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E31" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="F31" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E32" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="F32" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="E33" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="F33" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>298</v>
       </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4336,22 +4480,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.234375" customWidth="1"/>
-    <col min="2" max="2" width="28.41015625" customWidth="1"/>
-    <col min="3" max="3" width="19.234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>284</v>
       </c>
@@ -4365,7 +4509,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -4379,7 +4523,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -4393,7 +4537,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -4405,7 +4549,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
@@ -4417,7 +4561,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
@@ -4429,7 +4573,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
@@ -4443,7 +4587,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>202</v>
       </c>
@@ -4455,7 +4599,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>204</v>
       </c>
@@ -4469,7 +4613,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>207</v>
       </c>
@@ -4481,7 +4625,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>210</v>
       </c>
@@ -4493,7 +4637,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>213</v>
       </c>
@@ -4505,7 +4649,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>216</v>
       </c>
@@ -4517,7 +4661,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>219</v>
       </c>
@@ -4529,7 +4673,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
@@ -4541,7 +4685,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>225</v>
       </c>
@@ -4553,7 +4697,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>228</v>
       </c>
@@ -4565,7 +4709,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>231</v>
       </c>
@@ -4577,7 +4721,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>234</v>
       </c>
@@ -4589,7 +4733,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>237</v>
       </c>
@@ -4601,7 +4745,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
         <v>240</v>
       </c>
@@ -4613,7 +4757,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>243</v>
       </c>
@@ -4625,7 +4769,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>245</v>
       </c>
@@ -4637,7 +4781,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>247</v>
       </c>
@@ -4651,7 +4795,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>250</v>
       </c>
@@ -4663,7 +4807,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>253</v>
       </c>
@@ -4675,7 +4819,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>256</v>
       </c>
@@ -4689,7 +4833,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
         <v>259</v>
       </c>
@@ -4701,7 +4845,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>262</v>
       </c>
@@ -4715,7 +4859,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>265</v>
       </c>
@@ -4729,7 +4873,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>268</v>
       </c>
@@ -4741,7 +4885,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>271</v>
       </c>
@@ -4755,7 +4899,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>274</v>
       </c>
@@ -4769,7 +4913,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>277</v>
       </c>
@@ -4781,7 +4925,7 @@
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>280</v>
       </c>
@@ -4793,7 +4937,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
@@ -4805,7 +4949,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
         <v>182</v>
       </c>

</xml_diff>

<commit_message>
Added cache support for AKShareEquityHistoricalData
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6144" yWindow="204" windowWidth="12960" windowHeight="10968" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="6144" yWindow="204" windowWidth="12960" windowHeight="10968"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="630">
   <si>
     <t>Model</t>
   </si>
@@ -2371,9 +2371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2386,6 +2383,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2692,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2705,11 +2705,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="24" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1" t="s">
         <v>191</v>
       </c>
@@ -2907,7 +2907,9 @@
       <c r="F11" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
@@ -5246,7 +5248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -5467,38 +5469,38 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
         <v>629</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="14" t="s">
         <v>627</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18" t="s">
         <v>427</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22" t="s">
         <v>628</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated files in docs/
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D167BC26-922B-4B4C-A51F-F87EF1B8C414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6144" yWindow="204" windowWidth="12960" windowHeight="10968"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -26,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -119,12 +125,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roger Ye</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="635">
   <si>
     <t>Model</t>
   </si>
@@ -2148,17 +2154,37 @@
   </si>
   <si>
     <t>Need to remove</t>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateType</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optional[str]</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optional[int]</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optional[float]</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2166,7 +2192,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2198,7 +2224,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2207,7 +2233,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2216,7 +2242,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2224,7 +2250,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2350,7 +2376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2366,8 +2392,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2376,8 +2400,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -2388,7 +2411,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2404,9 +2427,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2444,7 +2467,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2516,7 +2539,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2689,32 +2712,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="D1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2733,11 +2756,11 @@
       <c r="F2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="2" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2756,7 +2779,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2775,7 +2798,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -2794,7 +2817,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -2813,7 +2836,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>400</v>
       </c>
@@ -2830,7 +2853,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>403</v>
       </c>
@@ -2844,7 +2867,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -2865,11 +2888,11 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>428</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>614</v>
       </c>
       <c r="C10" t="s">
@@ -2888,7 +2911,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -2911,7 +2934,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>194</v>
       </c>
@@ -2930,7 +2953,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>474</v>
       </c>
@@ -2940,13 +2963,13 @@
       <c r="C13" t="s">
         <v>607</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>185</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -2964,486 +2987,547 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A2:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.234375" customWidth="1"/>
+    <col min="3" max="3" width="28.41015625" customWidth="1"/>
+    <col min="4" max="4" width="19.234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>284</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>256</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -3453,20 +3537,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.64453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -3480,7 +3564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -3494,7 +3578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3508,7 +3592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -3516,7 +3600,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -3526,7 +3610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -3534,7 +3618,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -3542,7 +3626,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3559,27 +3643,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.87890625" customWidth="1"/>
+    <col min="6" max="6" width="22.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -3599,7 +3683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -3615,7 +3699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -3631,7 +3715,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -3647,7 +3731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>134</v>
       </c>
@@ -3661,7 +3745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>135</v>
       </c>
@@ -3675,7 +3759,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>136</v>
       </c>
@@ -3689,7 +3773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>137</v>
       </c>
@@ -3703,7 +3787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>138</v>
       </c>
@@ -3717,7 +3801,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>139</v>
       </c>
@@ -3731,7 +3815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>140</v>
       </c>
@@ -3745,7 +3829,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
@@ -3759,7 +3843,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>142</v>
       </c>
@@ -3773,7 +3857,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>143</v>
       </c>
@@ -3787,7 +3871,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>144</v>
       </c>
@@ -3801,7 +3885,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>145</v>
       </c>
@@ -3815,7 +3899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>146</v>
       </c>
@@ -3829,7 +3913,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>147</v>
       </c>
@@ -3843,7 +3927,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>148</v>
       </c>
@@ -3857,7 +3941,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>149</v>
       </c>
@@ -3871,7 +3955,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>150</v>
       </c>
@@ -3885,7 +3969,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -3899,7 +3983,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -3913,7 +3997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>153</v>
       </c>
@@ -3927,7 +4011,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>154</v>
       </c>
@@ -3941,7 +4025,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -3955,7 +4039,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -3969,7 +4053,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>157</v>
       </c>
@@ -3983,7 +4067,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>158</v>
       </c>
@@ -3997,7 +4081,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>159</v>
       </c>
@@ -4011,7 +4095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>160</v>
       </c>
@@ -4025,7 +4109,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -4039,7 +4123,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>162</v>
       </c>
@@ -4053,7 +4137,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>163</v>
       </c>
@@ -4067,7 +4151,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>164</v>
       </c>
@@ -4081,7 +4165,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>165</v>
       </c>
@@ -4095,7 +4179,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>166</v>
       </c>
@@ -4109,7 +4193,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>167</v>
       </c>
@@ -4123,7 +4207,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>168</v>
       </c>
@@ -4137,7 +4221,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>169</v>
       </c>
@@ -4151,7 +4235,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>170</v>
       </c>
@@ -4165,7 +4249,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>171</v>
       </c>
@@ -4179,7 +4263,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>173</v>
       </c>
@@ -4193,7 +4277,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>174</v>
       </c>
@@ -4207,7 +4291,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>175</v>
       </c>
@@ -4221,7 +4305,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
         <v>176</v>
       </c>
@@ -4235,7 +4319,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>177</v>
       </c>
@@ -4249,7 +4333,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>178</v>
       </c>
@@ -4263,7 +4347,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>179</v>
       </c>
@@ -4277,7 +4361,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>180</v>
       </c>
@@ -4291,7 +4375,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>181</v>
       </c>
@@ -4305,7 +4389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>129</v>
       </c>
@@ -4319,7 +4403,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -4340,21 +4424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="42.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -4368,7 +4452,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -4382,7 +4466,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -4396,7 +4480,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -4408,7 +4492,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
@@ -4420,7 +4504,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
@@ -4432,7 +4516,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
@@ -4446,7 +4530,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>393</v>
       </c>
@@ -4454,7 +4538,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>306</v>
       </c>
@@ -4466,7 +4550,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>240</v>
       </c>
@@ -4478,7 +4562,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>308</v>
       </c>
@@ -4490,7 +4574,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>311</v>
       </c>
@@ -4502,7 +4586,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>314</v>
       </c>
@@ -4514,7 +4598,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>317</v>
       </c>
@@ -4526,7 +4610,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>320</v>
       </c>
@@ -4538,7 +4622,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>322</v>
       </c>
@@ -4550,7 +4634,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>325</v>
       </c>
@@ -4562,7 +4646,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>328</v>
       </c>
@@ -4574,7 +4658,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>331</v>
       </c>
@@ -4586,7 +4670,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>394</v>
       </c>
@@ -4594,7 +4678,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>334</v>
       </c>
@@ -4606,7 +4690,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>337</v>
       </c>
@@ -4618,7 +4702,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>340</v>
       </c>
@@ -4630,7 +4714,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>343</v>
       </c>
@@ -4642,7 +4726,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>346</v>
       </c>
@@ -4654,7 +4738,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>349</v>
       </c>
@@ -4666,7 +4750,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>395</v>
       </c>
@@ -4674,7 +4758,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>352</v>
       </c>
@@ -4686,7 +4770,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>355</v>
       </c>
@@ -4698,7 +4782,7 @@
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>358</v>
       </c>
@@ -4710,7 +4794,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>361</v>
       </c>
@@ -4722,7 +4806,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>364</v>
       </c>
@@ -4734,7 +4818,7 @@
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>367</v>
       </c>
@@ -4746,7 +4830,7 @@
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>396</v>
       </c>
@@ -4754,7 +4838,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>370</v>
       </c>
@@ -4766,7 +4850,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>373</v>
       </c>
@@ -4778,7 +4862,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>376</v>
       </c>
@@ -4790,7 +4874,7 @@
       </c>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>379</v>
       </c>
@@ -4802,7 +4886,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>397</v>
       </c>
@@ -4810,7 +4894,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>382</v>
       </c>
@@ -4822,7 +4906,7 @@
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>385</v>
       </c>
@@ -4834,7 +4918,7 @@
       </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>388</v>
       </c>
@@ -4846,7 +4930,7 @@
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>398</v>
       </c>
@@ -4854,7 +4938,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>129</v>
       </c>
@@ -4866,7 +4950,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>182</v>
       </c>
@@ -4886,23 +4970,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -4919,7 +5003,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -4932,7 +5016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>406</v>
       </c>
@@ -4945,7 +5029,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>407</v>
       </c>
@@ -4958,7 +5042,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>408</v>
       </c>
@@ -4971,7 +5055,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>409</v>
       </c>
@@ -4982,7 +5066,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>410</v>
       </c>
@@ -4993,7 +5077,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>411</v>
       </c>
@@ -5004,7 +5088,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -5015,7 +5099,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5026,7 +5110,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>426</v>
       </c>
@@ -5037,7 +5121,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>424</v>
       </c>
@@ -5055,20 +5139,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -5085,7 +5169,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>415</v>
       </c>
@@ -5096,7 +5180,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>416</v>
       </c>
@@ -5107,7 +5191,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>426</v>
       </c>
@@ -5120,7 +5204,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>406</v>
       </c>
@@ -5133,7 +5217,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>407</v>
       </c>
@@ -5146,7 +5230,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>408</v>
       </c>
@@ -5159,7 +5243,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>409</v>
       </c>
@@ -5170,7 +5254,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>410</v>
       </c>
@@ -5181,7 +5265,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>417</v>
       </c>
@@ -5194,7 +5278,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -5205,7 +5289,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -5216,7 +5300,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" customHeight="1">
+    <row r="14" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6" t="s">
@@ -5227,7 +5311,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -5245,24 +5329,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>475</v>
       </c>
@@ -5282,7 +5366,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -5302,7 +5386,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>406</v>
       </c>
@@ -5322,7 +5406,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>407</v>
       </c>
@@ -5342,7 +5426,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>408</v>
       </c>
@@ -5362,7 +5446,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>409</v>
       </c>
@@ -5382,7 +5466,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>410</v>
       </c>
@@ -5402,7 +5486,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>411</v>
       </c>
@@ -5418,7 +5502,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>424</v>
       </c>
@@ -5434,7 +5518,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>425</v>
       </c>
@@ -5450,7 +5534,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>624</v>
       </c>
@@ -5468,41 +5552,39 @@
         <v>625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="12" t="s">
         <v>627</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="13" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="14"/>
+      <c r="E14" s="15" t="s">
         <v>427</v>
       </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22" t="s">
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
         <v>628</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="20"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5510,7 +5592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G49"/>
   <sheetViews>
@@ -5519,17 +5601,17 @@
       <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.52734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1171875" customWidth="1"/>
+    <col min="3" max="3" width="55.1171875" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1171875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>475</v>
       </c>
@@ -5552,7 +5634,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -5573,7 +5655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -5594,7 +5676,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>478</v>
       </c>
@@ -5611,7 +5693,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" hidden="1">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>479</v>
       </c>
@@ -5628,7 +5710,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>480</v>
       </c>
@@ -5645,7 +5727,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>481</v>
       </c>
@@ -5662,7 +5744,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>482</v>
       </c>
@@ -5679,7 +5761,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" hidden="1">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -5696,7 +5778,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>483</v>
       </c>
@@ -5713,7 +5795,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>485</v>
       </c>
@@ -5734,7 +5816,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>486</v>
       </c>
@@ -5755,7 +5837,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>487</v>
       </c>
@@ -5776,7 +5858,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>488</v>
       </c>
@@ -5797,7 +5879,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>489</v>
       </c>
@@ -5818,7 +5900,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>490</v>
       </c>
@@ -5839,7 +5921,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>491</v>
       </c>
@@ -5860,7 +5942,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>492</v>
       </c>
@@ -5877,7 +5959,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>493</v>
       </c>
@@ -5894,7 +5976,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>494</v>
       </c>
@@ -5911,7 +5993,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>495</v>
       </c>
@@ -5930,7 +6012,7 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>496</v>
       </c>
@@ -5949,7 +6031,7 @@
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>497</v>
       </c>
@@ -5968,7 +6050,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>498</v>
       </c>
@@ -5985,7 +6067,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>499</v>
       </c>
@@ -6002,7 +6084,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>500</v>
       </c>
@@ -6021,7 +6103,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>501</v>
       </c>
@@ -6038,7 +6120,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>502</v>
       </c>
@@ -6055,7 +6137,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>503</v>
       </c>
@@ -6072,7 +6154,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>505</v>
       </c>
@@ -6089,7 +6171,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>506</v>
       </c>
@@ -6108,7 +6190,7 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>507</v>
       </c>
@@ -6129,7 +6211,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>508</v>
       </c>
@@ -6146,7 +6228,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>509</v>
       </c>
@@ -6163,7 +6245,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>510</v>
       </c>
@@ -6180,7 +6262,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>512</v>
       </c>
@@ -6197,7 +6279,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>513</v>
       </c>
@@ -6214,7 +6296,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>514</v>
       </c>
@@ -6235,7 +6317,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>515</v>
       </c>
@@ -6252,7 +6334,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="8" t="s">
         <v>519</v>
       </c>
@@ -6271,7 +6353,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="8" t="s">
         <v>579</v>
       </c>
@@ -6288,7 +6370,7 @@
       </c>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="8" t="s">
         <v>580</v>
       </c>
@@ -6305,7 +6387,7 @@
       </c>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="8" t="s">
         <v>578</v>
       </c>
@@ -6324,7 +6406,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="8" t="s">
         <v>584</v>
       </c>
@@ -6343,7 +6425,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="8" t="s">
         <v>595</v>
       </c>
@@ -6362,7 +6444,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="8" t="s">
         <v>585</v>
       </c>
@@ -6379,7 +6461,7 @@
       </c>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="8" t="s">
         <v>596</v>
       </c>
@@ -6398,7 +6480,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="8" t="s">
         <v>9</v>
       </c>
@@ -6416,36 +6498,37 @@
       <c r="G49" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G49">
+  <autoFilter ref="A2:G49" xr:uid="{00000000-0009-0000-0000-000007000000}">
     <filterColumn colId="5">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.52734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>392</v>
       </c>
@@ -6465,7 +6548,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>429</v>
       </c>
@@ -6481,7 +6564,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>430</v>
       </c>
@@ -6493,7 +6576,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>431</v>
       </c>
@@ -6509,7 +6592,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>432</v>
       </c>
@@ -6521,7 +6604,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>433</v>
       </c>
@@ -6533,7 +6616,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>434</v>
       </c>
@@ -6545,7 +6628,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>435</v>
       </c>
@@ -6557,7 +6640,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>436</v>
       </c>
@@ -6569,7 +6652,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>437</v>
       </c>
@@ -6581,7 +6664,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>438</v>
       </c>
@@ -6593,7 +6676,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>439</v>
       </c>
@@ -6605,7 +6688,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>440</v>
       </c>
@@ -6617,7 +6700,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>441</v>
       </c>
@@ -6629,7 +6712,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>442</v>
       </c>
@@ -6641,7 +6724,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>443</v>
       </c>
@@ -6653,7 +6736,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>444</v>
       </c>
@@ -6665,7 +6748,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>445</v>
       </c>
@@ -6677,7 +6760,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>446</v>
       </c>
@@ -6689,7 +6772,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>447</v>
       </c>
@@ -6705,7 +6788,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>448</v>
       </c>
@@ -6717,7 +6800,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>449</v>
       </c>
@@ -6729,7 +6812,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>450</v>
       </c>
@@ -6741,7 +6824,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>451</v>
       </c>
@@ -6757,7 +6840,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>452</v>
       </c>
@@ -6773,7 +6856,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>453</v>
       </c>
@@ -6789,7 +6872,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>454</v>
       </c>
@@ -6801,7 +6884,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>455</v>
       </c>
@@ -6817,7 +6900,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>456</v>
       </c>
@@ -6829,7 +6912,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>457</v>
       </c>
@@ -6845,7 +6928,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>458</v>
       </c>
@@ -6861,7 +6944,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>459</v>
       </c>
@@ -6877,7 +6960,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>460</v>
       </c>
@@ -6889,7 +6972,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>461</v>
       </c>

</xml_diff>

<commit_message>
Fixed an issue in income_statement.py
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D167BC26-922B-4B4C-A51F-F87EF1B8C414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B3B69C-7C74-4D0C-B6A5-0D45BA448067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,6 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">EquityInfo!$A$2:$G$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">IncomeStatement!$A$2:$F$38</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -209,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="637">
   <si>
     <t>Model</t>
   </si>
@@ -2173,6 +2174,14 @@
   </si>
   <si>
     <t>Optional[float]</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2988,21 +2997,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A2:E38"/>
+  <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="29.234375" customWidth="1"/>
-    <col min="3" max="3" width="28.41015625" customWidth="1"/>
-    <col min="4" max="4" width="19.234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.234375" customWidth="1"/>
+    <col min="2" max="2" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.52734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.41015625" customWidth="1"/>
+    <col min="5" max="5" width="19.234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>284</v>
       </c>
@@ -3010,16 +3021,19 @@
         <v>630</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -3027,16 +3041,19 @@
         <v>631</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -3044,16 +3061,19 @@
         <v>632</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -3061,475 +3081,512 @@
         <v>633</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>216</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>219</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>225</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>228</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>237</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>240</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>243</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>253</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>256</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>259</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>277</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>280</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:F38" xr:uid="{00000000-0001-0000-0900-000000000000}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5598,7 +5655,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
@@ -5622,7 +5679,7 @@
         <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>635</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>516</v>

</xml_diff>

<commit_message>
Support income statement cache
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B3B69C-7C74-4D0C-B6A5-0D45BA448067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9004AB69-8A3D-4E86-B6CF-45982200EC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="637">
   <si>
     <t>Model</t>
   </si>
@@ -2724,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
@@ -2960,7 +2960,9 @@
         <v>298</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
@@ -2999,7 +3001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Local cache is enabled for cash flow report
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9004AB69-8A3D-4E86-B6CF-45982200EC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C9DD0-AE89-474C-AE28-94E40F805D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="637">
   <si>
     <t>Model</t>
   </si>
@@ -2725,7 +2725,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
@@ -2824,7 +2824,9 @@
         <v>185</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Local cache is enabled for balance sheet report
</commit_message>
<xml_diff>
--- a/docs/models.xlsx
+++ b/docs/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\tmp\akshare\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C9DD0-AE89-474C-AE28-94E40F805D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8F23FA-48DE-458A-AD59-1AE61A73DF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="637">
   <si>
     <t>Model</t>
   </si>
@@ -2725,7 +2725,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.4"/>
@@ -2805,7 +2805,9 @@
         <v>185</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -2897,7 +2899,9 @@
       <c r="F9" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
@@ -2941,9 +2945,7 @@
       <c r="F11" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>185</v>
-      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">

</xml_diff>